<commit_message>
updated template files, added warning
</commit_message>
<xml_diff>
--- a/Templates/student.xlsx
+++ b/Templates/student.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>First Name</t>
   </si>
@@ -50,6 +50,72 @@
   </si>
   <si>
     <t>Effort Level</t>
+  </si>
+  <si>
+    <t>Jessie</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Self Management</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Thinking</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Uzen</t>
+  </si>
+  <si>
+    <t>Huang</t>
+  </si>
+  <si>
+    <t>Edwin</t>
+  </si>
+  <si>
+    <t>Kung</t>
+  </si>
+  <si>
+    <t>Irina</t>
+  </si>
+  <si>
+    <t>Qiu</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jessie </t>
+  </si>
+  <si>
+    <t>Chen</t>
+  </si>
+  <si>
+    <t>Research</t>
   </si>
 </sst>
 </file>
@@ -216,7 +282,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -226,22 +292,28 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1337,9 +1409,9 @@
     <col min="3" max="6" width="8.35156" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.7266" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.35156" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.61719" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.46094" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.0469" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5781" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.3359" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.03125" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.35156" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.3594" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.35156" style="1" customWidth="1"/>
@@ -1387,94 +1459,250 @@
       </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="A2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="M2" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="A3" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="M3" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="A4" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9">
+        <v>4</v>
+      </c>
+      <c r="F4" s="9">
+        <v>8</v>
+      </c>
+      <c r="G4" s="9">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s" s="10">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="L4" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="M4" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="A5" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="M5" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="A6" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="C6" s="9">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9">
+        <v>6</v>
+      </c>
+      <c r="E6" s="9">
+        <v>7</v>
+      </c>
+      <c r="F6" s="9">
+        <v>8</v>
+      </c>
+      <c r="G6" s="9">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="M6" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="A7" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="C7" s="9">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9">
+        <v>8</v>
+      </c>
+      <c r="E7" s="9">
+        <v>8</v>
+      </c>
+      <c r="F7" s="9">
+        <v>7</v>
+      </c>
+      <c r="G7" s="9">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="L7" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="M7" s="9">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>